<commit_message>
Cambio encoding y directorios de imput y output
</commit_message>
<xml_diff>
--- a/src/exp_colectivo/secuencia.xlsx
+++ b/src/exp_colectivo/secuencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgaricoche\Desktop\Facultad\DMEyF_2022\repo\dmeyf_2022\src\exp_colectivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DD9061-BC21-4481-A313-5ACA59DDDB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F795CDA-28B6-4703-8E85-C1A817DA99D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{66CD2E9A-68E3-4D6A-AA2B-036C42E09D3A}"/>
   </bookViews>
@@ -104,21 +104,12 @@
     <t>Machine Learing</t>
   </si>
   <si>
-    <t>exp/EC/CA9060/dataset.csv.gz</t>
-  </si>
-  <si>
     <t>Corregir drifting</t>
   </si>
   <si>
     <t>Rank cero fijo.</t>
   </si>
   <si>
-    <t>exp/EC/DR9141/dataset.csv.gz</t>
-  </si>
-  <si>
-    <t>exp/EC/FE9251/dataset.csv.gz</t>
-  </si>
-  <si>
     <t>Canarios asesinos</t>
   </si>
   <si>
@@ -132,6 +123,15 @@
   </si>
   <si>
     <t>Duración</t>
+  </si>
+  <si>
+    <t>exp/EC_CA9060/dataset.csv.gz</t>
+  </si>
+  <si>
+    <t>exp/EC_DR9141/dataset.csv.gz</t>
+  </si>
+  <si>
+    <t>exp/EC_FE9251/dataset.csv.gz</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <dimension ref="A2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +531,7 @@
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -548,7 +548,7 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
@@ -556,41 +556,41 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4">
         <v>914</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>925</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -635,7 +635,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Agrego TS y BO
</commit_message>
<xml_diff>
--- a/src/exp_colectivo/secuencia.xlsx
+++ b/src/exp_colectivo/secuencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgaricoche\Desktop\Facultad\DMEyF_2022\repo\dmeyf_2022\src\exp_colectivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F795CDA-28B6-4703-8E85-C1A817DA99D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4DD448-E2ED-4590-B2ED-D7638F52D860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{66CD2E9A-68E3-4D6A-AA2B-036C42E09D3A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>HECHO</t>
   </si>
@@ -68,39 +68,12 @@
     <t>datasets/competencia3_2022.csv.gz</t>
   </si>
   <si>
-    <t>Todos menos los obvios</t>
-  </si>
-  <si>
-    <t>exp/FE9251/dataset.csv.gz</t>
-  </si>
-  <si>
     <t>Rank para tratar Data Drifting</t>
   </si>
   <si>
-    <t>Campos monetarios (frank con cero)</t>
-  </si>
-  <si>
     <t>914_2</t>
   </si>
   <si>
-    <t>exp/DR9142/dataset.csv.gz</t>
-  </si>
-  <si>
-    <t>Se colgó con 256 gigas de ram</t>
-  </si>
-  <si>
-    <t>Lags, delta lags y tendencias. Canarios asesinos</t>
-  </si>
-  <si>
-    <t>925_2</t>
-  </si>
-  <si>
-    <t>exp/FE9252/dataset.csv.gz</t>
-  </si>
-  <si>
-    <t>Consumió 500 gigas de ram. Dejó 1896 vbles</t>
-  </si>
-  <si>
     <t>Machine Learing</t>
   </si>
   <si>
@@ -110,9 +83,6 @@
     <t>Rank cero fijo.</t>
   </si>
   <si>
-    <t>Canarios asesinos</t>
-  </si>
-  <si>
     <t>FE histórico y canarios</t>
   </si>
   <si>
@@ -132,6 +102,67 @@
   </si>
   <si>
     <t>exp/EC_FE9251/dataset.csv.gz</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>2 minutos</t>
+  </si>
+  <si>
+    <t>Training strategy</t>
+  </si>
+  <si>
+    <t>914_1</t>
+  </si>
+  <si>
+    <t>exp/EC_TS931_1/dataset.csv.gz</t>
+  </si>
+  <si>
+    <t>10 minutos</t>
+  </si>
+  <si>
+    <t>exp/EC_TS931_2/dataset.csv.gz</t>
+  </si>
+  <si>
+    <t>train &amp; final_train: jun-19 a dic-19 y sep-20 a ene-21
+validation: feb-21
+test: may-19 y may-21
+seed: 335897
+undersampling: 0.4</t>
+  </si>
+  <si>
+    <t>15 minutos</t>
+  </si>
+  <si>
+    <t>Canarios asesinos. 257 variables finales</t>
+  </si>
+  <si>
+    <t>train &amp; final_train: may-19 a dic-19 y sep-20 a ene-21
+validation: feb-21
+test: mar-21, abr-21, may-21.
+seed: 335897
+undersampling: 0.4</t>
+  </si>
+  <si>
+    <t>BO</t>
+  </si>
+  <si>
+    <t>exp/EC_HT9420_1/dataset.csv.gz</t>
+  </si>
+  <si>
+    <t>Undersampling aplicado.
+KBO_iteraciones: 100
+seed: 335897</t>
+  </si>
+  <si>
+    <t>942_1</t>
+  </si>
+  <si>
+    <t>942_2</t>
+  </si>
+  <si>
+    <t>exp/EC_HT9420_2/dataset.csv.gz</t>
   </si>
 </sst>
 </file>
@@ -175,9 +206,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB7E0C5-F25A-4B1D-8DDE-18F7D275B2D4}">
-  <dimension ref="A2:H13"/>
+  <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,8 +538,9 @@
     <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -531,10 +566,13 @@
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -548,134 +586,137 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>914</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>925</v>
       </c>
       <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="G10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
         <v>11</v>
       </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" t="s">
-        <v>20</v>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambio cortes hasta los 15.000
</commit_message>
<xml_diff>
--- a/src/exp_colectivo/secuencia.xlsx
+++ b/src/exp_colectivo/secuencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgaricoche\Desktop\Facultad\DMEyF_2022\repo\dmeyf_2022\src\exp_colectivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F5A167-4635-4DFC-8BF3-64FAFE6E2ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD64F45B-00E7-4551-A9E1-AD024F8B7182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{66CD2E9A-68E3-4D6A-AA2B-036C42E09D3A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>HECHO</t>
   </si>
@@ -186,7 +186,11 @@
     <t>exp/EC_ZZ9420_2/dataset.csv.gz</t>
   </si>
   <si>
-    <t>seeds: c(335897, 679909, 320923, 629243, 659819)</t>
+    <t>7 horas y 30 minutos</t>
+  </si>
+  <si>
+    <t>seeds: c(335897, 679909, 320923, 629243, 659819)
+Corte: 7000 a 15000</t>
   </si>
 </sst>
 </file>
@@ -552,7 +556,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB7E0C5-F25A-4B1D-8DDE-18F7D275B2D4}">
   <dimension ref="A2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -714,7 +720,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>41</v>
       </c>
@@ -727,8 +733,8 @@
       <c r="F12" t="s">
         <v>44</v>
       </c>
-      <c r="G12" t="s">
-        <v>46</v>
+      <c r="G12" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -759,7 +765,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -775,8 +784,11 @@
       <c r="G17" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>41</v>
       </c>
@@ -789,8 +801,8 @@
       <c r="F18" t="s">
         <v>45</v>
       </c>
-      <c r="G18" t="s">
-        <v>46</v>
+      <c r="G18" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>